<commit_message>
change teacher basic info data from month to year
</commit_message>
<xml_diff>
--- a/web/src/main/resources/static/excel/teacher-furtherInfo.xlsx
+++ b/web/src/main/resources/static/excel/teacher-furtherInfo.xlsx
@@ -28,7 +28,7 @@
     <t xml:space="preserve">پایه</t>
   </si>
   <si>
-    <t xml:space="preserve">سابقه(ماه)</t>
+    <t xml:space="preserve">سابقه(سال)</t>
   </si>
   <si>
     <t xml:space="preserve">رتبه</t>
@@ -157,7 +157,7 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="true" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
+      <selection pane="topLeft" activeCell="L9" activeCellId="0" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -183,11 +183,7 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="6">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C1" type="whole">
-      <formula1>0</formula1>
-      <formula2>1E+034</formula2>
-    </dataValidation>
+  <dataValidations count="5">
     <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B1" type="whole">
       <formula1>0</formula1>
       <formula2>1E+035</formula2>
@@ -200,13 +196,13 @@
       <formula1>0</formula1>
       <formula2>1E+035</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C2:C1001" type="whole">
-      <formula1>0</formula1>
-      <formula2>1E+034</formula2>
-    </dataValidation>
     <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D2:D1001" type="list">
       <formula1>"استاد,دانشیار,استادیار,مربی,آموزشیار"</formula1>
       <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C1:C1001" type="whole">
+      <formula1>0</formula1>
+      <formula2>1E+034</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>